<commit_message>
Bivariate distribution informed by GTEx data
reading_gtex.py - reads files from external directory and processes the them to get bivariate distributions for mRNA transcripts
setup.py - builds a long table out of all simulations. Error at saving to file
correct_model.py - uses the GTEx infromed distribution to generate conductance multipliers.
</commit_message>
<xml_diff>
--- a/Eichel etal data/elife-52654-fig7-data3-v2.xlsx
+++ b/Eichel etal data/elife-52654-fig7-data3-v2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/PyCharm/Channel_coexpression/Eichel etal data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{167086E6-B6CF-8343-A75F-700D044FC99E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7C997D-C521-BF43-8B53-7AB3B5F85E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" activeTab="1" xr2:uid="{35307B67-0046-7D48-BE7F-98A5F8DF35A3}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{35307B67-0046-7D48-BE7F-98A5F8DF35A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 7d" sheetId="1" r:id="rId1"/>
     <sheet name="Figure 7e" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,15 +24,42 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>x</t>
   </si>
@@ -77,6 +104,15 @@
   </si>
   <si>
     <t>Control</t>
+  </si>
+  <si>
+    <t>Avg difference</t>
+  </si>
+  <si>
+    <t>diff in decimals</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -140,7 +176,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4254500" cy="3403600"/>
+    <xdr:ext cx="4251960" cy="3401568"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
@@ -169,7 +205,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9906000" y="609600"/>
-          <a:ext cx="4254500" cy="3403600"/>
+          <a:ext cx="4251960" cy="3401568"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -232,7 +268,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -528,15 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888B4650-E0D8-DF49-96F8-4CA99329F93F}">
-  <dimension ref="B2:K22"/>
+  <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>14</v>
       </c>
@@ -564,8 +603,11 @@
       <c r="K2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-50</v>
       </c>
@@ -593,8 +635,12 @@
       <c r="K3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L3" cm="1">
+        <f t="array" ref="L3:L11">I3:I11-I14:I22</f>
+        <v>1.1680128712517081E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-40</v>
       </c>
@@ -622,8 +668,11 @@
       <c r="K4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>3.4515578811988259E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>-30</v>
       </c>
@@ -651,8 +700,11 @@
       <c r="K5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>1.4188518375158166E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>-20</v>
       </c>
@@ -680,8 +732,11 @@
       <c r="K6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>9.395233318209617E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>-10</v>
       </c>
@@ -709,8 +764,11 @@
       <c r="K7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>0.17350140511989592</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>0</v>
       </c>
@@ -738,8 +796,11 @@
       <c r="K8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>0.18740733563899964</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>10</v>
       </c>
@@ -767,8 +828,11 @@
       <c r="K9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>0.2643748197238891</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>20</v>
       </c>
@@ -796,8 +860,11 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>0.3091431833337992</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>30</v>
       </c>
@@ -822,8 +889,11 @@
       <c r="K11">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>0.55273064039647601</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -849,7 +919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>-50</v>
       </c>
@@ -875,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>-40</v>
       </c>
@@ -901,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>-30</v>
       </c>
@@ -1081,6 +1151,57 @@
       </c>
       <c r="K22">
         <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I25" cm="1">
+        <f t="array" ref="I25:I33">(I14:I22)/I3:I11</f>
+        <v>1.952248780872744</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>0.47034359375173684</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>0.9090688099008436</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>0.68098120650034288</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>0.59647552202599974</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>0.5800199096520563</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>0.38153901279942143</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>0.33071512341588594</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>1.1979771371032469E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1091,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144EC616-E4F2-C84B-A2CE-B23B575FA523}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,6 +1660,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I21" cm="1">
+        <f t="array" ref="I21:I27">(I12:I18)/I3:I9</f>
+        <v>-1.7697452357799695</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>1.2942609467728654</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>0.51517981571435223</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>0.31984352092732532</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>0.4470962733804496</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>0.4497553297879735</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>0.32401288190875971</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
intermediate report - diagramme under "wrong" assumption
</commit_message>
<xml_diff>
--- a/Eichel etal data/elife-52654-fig7-data3-v2.xlsx
+++ b/Eichel etal data/elife-52654-fig7-data3-v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/Projects/PyCharm/Channel_coexpression/Eichel etal data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/PyCharm/Channel_coexpression/Eichel etal data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9207041D-9555-734F-A7AD-138C423BD256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0FA7CB-AECC-F64E-971D-45FB672CC075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{35307B67-0046-7D48-BE7F-98A5F8DF35A3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{35307B67-0046-7D48-BE7F-98A5F8DF35A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 7d" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>x</t>
   </si>
@@ -112,7 +112,13 @@
     <t>diff in decimals</t>
   </si>
   <si>
-    <t>diff</t>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>avg fraction</t>
+  </si>
+  <si>
+    <t>avg_fraction</t>
   </si>
 </sst>
 </file>
@@ -128,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +144,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,9 +166,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,7 +246,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3522579" cy="2755900"/>
+    <xdr:ext cx="3518034" cy="2752344"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
@@ -262,7 +275,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9905999" y="609600"/>
-          <a:ext cx="3522579" cy="2755900"/>
+          <a:ext cx="3518034" cy="2752344"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -571,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888B4650-E0D8-DF49-96F8-4CA99329F93F}">
-  <dimension ref="B2:L33"/>
+  <dimension ref="B2:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,9 +1223,18 @@
         <v>0.33071512341588594</v>
       </c>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
       <c r="I33">
         <v>1.1979771371032469E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="2">
+        <f>AVERAGE(I26:I32)</f>
+        <v>0.5641633111494696</v>
       </c>
     </row>
   </sheetData>
@@ -1223,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144EC616-E4F2-C84B-A2CE-B23B575FA523}">
-  <dimension ref="B2:K27"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1712,6 +1734,15 @@
         <v>0.32401288190875971</v>
       </c>
     </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="2">
+        <f>AVERAGE(I23:I27)</f>
+        <v>0.41117756434377206</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>